<commit_message>
added some more cards that should be partially implemented based on others with the same effect working
</commit_message>
<xml_diff>
--- a/CardCheckOff.xlsx
+++ b/CardCheckOff.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Documents\GitHub\RIT-Resilience-Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECAB4884-0C35-487F-B1D9-4BA8EF98EC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3087E3-5F2C-4316-94EA-E96B89499BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="2090" windowWidth="29480" windowHeight="19500" xr2:uid="{64B1DE55-618D-485E-BD09-95462C47B966}"/>
+    <workbookView xWindow="1550" yWindow="1760" windowWidth="29480" windowHeight="19500" xr2:uid="{64B1DE55-618D-485E-BD09-95462C47B966}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="66">
   <si>
     <t>Quick Meeting</t>
   </si>
@@ -230,7 +230,26 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Only reduces 1 of them, isnt shown across on opponent UI</t>
+    <t>Applies the fortify effect, Need to implement fortify: This effect blocks the first red card effect and any active red effect that targets the facility that this effect is attached to. This includes the backdoor effect. This effect lasts for 3 turns.</t>
+  </si>
+  <si>
+    <t>Assumed because other card works</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Only reduces 1 of them, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>isnt shown across on opponent UI</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -288,21 +307,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -321,13 +326,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
         </patternFill>
       </fill>
     </dxf>
@@ -671,7 +669,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -791,10 +789,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
         <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>64</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
@@ -806,12 +807,14 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" t="s">
+        <v>64</v>
+      </c>
       <c r="E8">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -822,10 +825,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
         <v>42</v>
+      </c>
+      <c r="D9" t="s">
+        <v>64</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
@@ -853,10 +859,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
         <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
@@ -868,12 +877,14 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" t="s">
+        <v>64</v>
+      </c>
       <c r="E12">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -884,10 +895,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
         <v>46</v>
+      </c>
+      <c r="D13" t="s">
+        <v>63</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
@@ -1029,7 +1043,7 @@
         <v>53</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
@@ -1072,10 +1086,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C25" t="s">
         <v>56</v>
+      </c>
+      <c r="D25" t="s">
+        <v>64</v>
       </c>
       <c r="E25">
         <f t="shared" si="0"/>
@@ -1163,13 +1180,13 @@
   </sheetData>
   <autoFilter ref="E1:E30" xr:uid="{72602A32-B298-4D25-8C38-8BE194D72840}"/>
   <conditionalFormatting sqref="B2:B30">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>$G$1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>$G$2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>$G$3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
basic alert popup frame to display messages to a single player (discard or something)
</commit_message>
<xml_diff>
--- a/CardCheckOff.xlsx
+++ b/CardCheckOff.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Documents\GitHub\RIT-Resilience-Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA70B08-F3FE-4AAD-B3B5-7D1E0642C74D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07971BB-0116-4574-AA9D-F2492C1AA92F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9690" yWindow="520" windowWidth="28290" windowHeight="19200" xr2:uid="{64B1DE55-618D-485E-BD09-95462C47B966}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$F$1:$F$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="67">
   <si>
     <t>Quick Meeting</t>
   </si>
@@ -131,9 +131,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Working?</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -237,6 +234,12 @@
   </si>
   <si>
     <t>Can play on self</t>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
+    <t>Local</t>
   </si>
 </sst>
 </file>
@@ -653,531 +656,621 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72602A32-B298-4D25-8C38-8BE194D72840}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="3" max="3" width="134.1796875" customWidth="1"/>
-    <col min="4" max="4" width="47.6328125" customWidth="1"/>
+    <col min="4" max="4" width="134.1796875" customWidth="1"/>
+    <col min="5" max="5" width="47.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1">
+        <f>MOD(ROW(),2)</f>
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E1">
-        <f>MOD(ROW(),2)</f>
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2">
+        <f t="shared" ref="F2:F30" si="0">MOD(ROW(),2)</f>
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="2" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2">
-        <f t="shared" ref="E2:E30" si="0">MOD(ROW(),2)</f>
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="E3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" t="s">
-        <v>50</v>
+        <v>31</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>65</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+      <c r="E17" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" t="s">
-        <v>52</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="2"/>
-      <c r="E20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" t="s">
-        <v>36</v>
+        <v>31</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="D21" t="s">
-        <v>64</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="E21" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="2"/>
-      <c r="E22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" t="s">
-        <v>58</v>
-      </c>
-      <c r="E27">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" t="s">
+        <v>57</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" t="s">
-        <v>60</v>
-      </c>
-      <c r="E29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D30" s="2"/>
-      <c r="E30">
+        <v>30</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="2"/>
+      <c r="F30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E1:E30" xr:uid="{72602A32-B298-4D25-8C38-8BE194D72840}"/>
-  <conditionalFormatting sqref="B2:B30">
+  <autoFilter ref="F1:F30" xr:uid="{72602A32-B298-4D25-8C38-8BE194D72840}"/>
+  <conditionalFormatting sqref="B2:C30">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>$G$3</formula>
+      <formula>$H$3</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>$G$2</formula>
+      <formula>$H$2</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
-      <formula>$G$1</formula>
+      <formula>$H$1</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B30" xr:uid="{A9FEB94B-49B1-4D20-A169-0614241C47CC}">
-      <formula1>$G$1:$G$3</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C30" xr:uid="{A9FEB94B-49B1-4D20-A169-0614241C47CC}">
+      <formula1>$H$1:$H$3</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
more card actions, 13/29 fully done
</commit_message>
<xml_diff>
--- a/CardCheckOff.xlsx
+++ b/CardCheckOff.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Documents\GitHub\RIT-Resilience-Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07971BB-0116-4574-AA9D-F2492C1AA92F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A9CFCB-5BC0-434C-903E-C5D3E018EB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9690" yWindow="520" windowWidth="28290" windowHeight="19200" xr2:uid="{64B1DE55-618D-485E-BD09-95462C47B966}"/>
+    <workbookView xWindow="9690" yWindow="540" windowWidth="28230" windowHeight="19170" xr2:uid="{64B1DE55-618D-485E-BD09-95462C47B966}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="68">
   <si>
     <t>Quick Meeting</t>
   </si>
@@ -240,6 +240,9 @@
   </si>
   <si>
     <t>Local</t>
+  </si>
+  <si>
+    <t>No Card draw message?</t>
   </si>
 </sst>
 </file>
@@ -659,7 +662,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -701,12 +704,14 @@
         <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="F2">
         <f t="shared" ref="F2:F30" si="0">MOD(ROW(),2)</f>
         <v>0</v>
@@ -720,16 +725,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="D3" t="s">
         <v>35</v>
       </c>
-      <c r="E3" t="s">
-        <v>63</v>
+      <c r="E3" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="F3">
         <f t="shared" si="0"/>
@@ -744,16 +749,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
@@ -765,13 +770,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
organize card player cause i kept losing functions
</commit_message>
<xml_diff>
--- a/CardCheckOff.xlsx
+++ b/CardCheckOff.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Documents\GitHub\RIT-Resilience-Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A9CFCB-5BC0-434C-903E-C5D3E018EB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F9A496-904D-4B8C-8B8B-850ECCF15E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9690" yWindow="540" windowWidth="28230" windowHeight="19170" xr2:uid="{64B1DE55-618D-485E-BD09-95462C47B966}"/>
   </bookViews>
@@ -665,14 +665,14 @@
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="4" max="4" width="134.1796875" customWidth="1"/>
-    <col min="5" max="5" width="47.6328125" customWidth="1"/>
+    <col min="4" max="4" width="134.140625" customWidth="1"/>
+    <col min="5" max="5" width="47.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
@@ -696,7 +696,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -704,7 +704,7 @@
         <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>34</v>
@@ -720,7 +720,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -728,7 +728,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
         <v>35</v>
@@ -744,7 +744,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -765,7 +765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -786,7 +786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -805,7 +805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -823,7 +823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -842,7 +842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -860,7 +860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -879,7 +879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -897,7 +897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -916,7 +916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -934,7 +934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -953,7 +953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -971,7 +971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -992,7 +992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
working on effect ui
</commit_message>
<xml_diff>
--- a/CardCheckOff.xlsx
+++ b/CardCheckOff.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Documents\GitHub\RIT-Resilience-Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F9A496-904D-4B8C-8B8B-850ECCF15E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93BE83C-EAE4-429D-B8DF-5A8AA7CC55A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9690" yWindow="540" windowWidth="28230" windowHeight="19170" xr2:uid="{64B1DE55-618D-485E-BD09-95462C47B966}"/>
+    <workbookView xWindow="57495" yWindow="11010" windowWidth="21810" windowHeight="24375" xr2:uid="{64B1DE55-618D-485E-BD09-95462C47B966}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -185,12 +185,6 @@
     <t>Remove up to 2 red effects from your facilities.</t>
   </si>
   <si>
-    <t xml:space="preserve">If the Doom clock is active you can target an allied facility if not then target one of your facilities. Restore 1 Physical; Network; and Financial point on the targeted facility. </t>
-  </si>
-  <si>
-    <t>If the Doom clock is active you can add the Fortified effect to an allied facility.  If not then you can add the Fortified effect to one of your facilities.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Remove an effect on 1 facility. This card can target an allied facility as well if the Doom clock is active. </t>
   </si>
   <si>
@@ -230,9 +224,6 @@
     <t>Assumed because other card works</t>
   </si>
   <si>
-    <t>Draw works</t>
-  </si>
-  <si>
     <t>Can play on self</t>
   </si>
   <si>
@@ -243,6 +234,15 @@
   </si>
   <si>
     <t>No Card draw message?</t>
+  </si>
+  <si>
+    <t>If DC you can add the Fortified effect to an allied facility.  If not then you can add the Fortified effect to one of your facilities.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If DC active you can target an allied facility if not then target one of your facilities. Restore 1 of each point on the targeted facility. </t>
+  </si>
+  <si>
+    <t>not updating discard correctly in hands</t>
   </si>
 </sst>
 </file>
@@ -662,31 +662,31 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="4" max="4" width="134.140625" customWidth="1"/>
-    <col min="5" max="5" width="47.5703125" customWidth="1"/>
+    <col min="4" max="4" width="109.6328125" customWidth="1"/>
+    <col min="5" max="5" width="47.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F1">
         <f>MOD(ROW(),2)</f>
@@ -696,7 +696,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -710,7 +710,7 @@
         <v>34</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F2">
         <f t="shared" ref="F2:F30" si="0">MOD(ROW(),2)</f>
@@ -720,7 +720,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -734,7 +734,7 @@
         <v>35</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F3">
         <f t="shared" si="0"/>
@@ -744,7 +744,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -758,14 +758,14 @@
         <v>36</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -779,14 +779,14 @@
         <v>37</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -805,7 +805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -823,7 +823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -842,7 +842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -860,7 +860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -879,7 +879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -897,7 +897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -916,7 +916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -934,7 +934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -953,7 +953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -971,7 +971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -982,17 +982,17 @@
         <v>30</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1003,17 +1003,17 @@
         <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="E17" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>30</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18">
@@ -1032,7 +1032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1043,14 +1043,14 @@
         <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>32</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>34</v>
@@ -1069,28 +1069,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D21" t="s">
         <v>35</v>
       </c>
       <c r="E21" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F21">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>32</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22">
@@ -1109,7 +1109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1120,14 +1120,14 @@
         <v>30</v>
       </c>
       <c r="D23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -1138,17 +1138,17 @@
         <v>30</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1159,14 +1159,14 @@
         <v>30</v>
       </c>
       <c r="D25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F25">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
@@ -1177,17 +1177,17 @@
         <v>30</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1198,14 +1198,14 @@
         <v>30</v>
       </c>
       <c r="D27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F27">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
@@ -1216,17 +1216,17 @@
         <v>30</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1237,14 +1237,14 @@
         <v>30</v>
       </c>
       <c r="D29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F29">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>30</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30">

</xml_diff>

<commit_message>
fortify and blue remove effect work to remove backdoors, check off some more card actions
</commit_message>
<xml_diff>
--- a/CardCheckOff.xlsx
+++ b/CardCheckOff.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Documents\GitHub\RIT-Resilience-Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93BE83C-EAE4-429D-B8DF-5A8AA7CC55A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C0A63A-0258-488F-A5DD-2F1921B49EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57495" yWindow="11010" windowWidth="21810" windowHeight="24375" xr2:uid="{64B1DE55-618D-485E-BD09-95462C47B966}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{64B1DE55-618D-485E-BD09-95462C47B966}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="66">
   <si>
     <t>Quick Meeting</t>
   </si>
@@ -221,9 +221,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Assumed because other card works</t>
-  </si>
-  <si>
     <t>Can play on self</t>
   </si>
   <si>
@@ -233,16 +230,13 @@
     <t>Local</t>
   </si>
   <si>
-    <t>No Card draw message?</t>
-  </si>
-  <si>
     <t>If DC you can add the Fortified effect to an allied facility.  If not then you can add the Fortified effect to one of your facilities.</t>
   </si>
   <si>
     <t xml:space="preserve">If DC active you can target an allied facility if not then target one of your facilities. Restore 1 of each point on the targeted facility. </t>
   </si>
   <si>
-    <t>not updating discard correctly in hands</t>
+    <t>Return card to hand message</t>
   </si>
 </sst>
 </file>
@@ -266,7 +260,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,6 +270,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,10 +292,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,7 +663,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -677,10 +678,10 @@
         <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>33</v>
@@ -709,9 +710,7 @@
       <c r="D2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>64</v>
-      </c>
+      <c r="E2" s="2"/>
       <c r="F2">
         <f t="shared" ref="F2:F30" si="0">MOD(ROW(),2)</f>
         <v>0</v>
@@ -733,9 +732,7 @@
       <c r="D3" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>64</v>
-      </c>
+      <c r="E3" s="3"/>
       <c r="F3">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -758,7 +755,7 @@
         <v>36</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
@@ -778,8 +775,8 @@
       <c r="D5" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>64</v>
+      <c r="E5" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
@@ -813,7 +810,7 @@
         <v>32</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
         <v>39</v>
@@ -831,7 +828,7 @@
         <v>32</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>40</v>
@@ -850,7 +847,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
         <v>41</v>
@@ -887,7 +884,7 @@
         <v>32</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
         <v>43</v>
@@ -905,7 +902,7 @@
         <v>32</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>44</v>
@@ -924,7 +921,7 @@
         <v>32</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
         <v>45</v>
@@ -982,10 +979,10 @@
         <v>30</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
@@ -1003,10 +1000,10 @@
         <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
@@ -1018,10 +1015,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>48</v>
@@ -1082,9 +1079,6 @@
       <c r="D21" t="s">
         <v>35</v>
       </c>
-      <c r="E21" t="s">
-        <v>67</v>
-      </c>
       <c r="F21">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1132,17 +1126,15 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>60</v>
-      </c>
+      <c r="E24" s="2"/>
       <c r="F24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1156,7 +1148,7 @@
         <v>32</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D25" t="s">
         <v>53</v>
@@ -1171,17 +1163,15 @@
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>60</v>
-      </c>
+      <c r="E26" s="2"/>
       <c r="F26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1218,9 +1208,7 @@
       <c r="D28" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>60</v>
-      </c>
+      <c r="E28" s="2"/>
       <c r="F28">
         <f t="shared" si="0"/>
         <v>0</v>

</xml_diff>

<commit_message>
Threat Hunting card effect (remove effect from multi facility) works locally
</commit_message>
<xml_diff>
--- a/CardCheckOff.xlsx
+++ b/CardCheckOff.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Documents\GitHub\RIT-Resilience-Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C0A63A-0258-488F-A5DD-2F1921B49EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3B50B2-4F11-41F1-8E7F-84DC0FBB24F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{64B1DE55-618D-485E-BD09-95462C47B966}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="34240" windowHeight="20960" xr2:uid="{64B1DE55-618D-485E-BD09-95462C47B966}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -182,9 +182,6 @@
     <t>Fortify and restore 1 network point on 2 facilities in your sector.</t>
   </si>
   <si>
-    <t>Remove up to 2 red effects from your facilities.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Remove an effect on 1 facility. This card can target an allied facility as well if the Doom clock is active. </t>
   </si>
   <si>
@@ -237,6 +234,9 @@
   </si>
   <si>
     <t>Return card to hand message</t>
+  </si>
+  <si>
+    <t>Choose 2 of your facilities to remove Backdoor from.</t>
   </si>
 </sst>
 </file>
@@ -663,7 +663,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -678,16 +678,16 @@
         <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F1">
         <f>MOD(ROW(),2)</f>
@@ -755,7 +755,7 @@
         <v>36</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
@@ -776,7 +776,7 @@
         <v>37</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
@@ -955,13 +955,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
@@ -979,10 +979,10 @@
         <v>30</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
@@ -1000,10 +1000,10 @@
         <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
@@ -1021,7 +1021,7 @@
         <v>32</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18">
@@ -1040,7 +1040,7 @@
         <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
@@ -1095,7 +1095,7 @@
         <v>32</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22">
@@ -1114,7 +1114,7 @@
         <v>30</v>
       </c>
       <c r="D23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
@@ -1132,7 +1132,7 @@
         <v>32</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24">
@@ -1151,7 +1151,7 @@
         <v>32</v>
       </c>
       <c r="D25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F25">
         <f t="shared" si="0"/>
@@ -1169,7 +1169,7 @@
         <v>32</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26">
@@ -1188,7 +1188,7 @@
         <v>30</v>
       </c>
       <c r="D27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F27">
         <f t="shared" si="0"/>
@@ -1206,7 +1206,7 @@
         <v>30</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28">
@@ -1225,7 +1225,7 @@
         <v>30</v>
       </c>
       <c r="D29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F29">
         <f t="shared" si="0"/>
@@ -1243,7 +1243,7 @@
         <v>30</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30">

</xml_diff>

<commit_message>
got multi facility effect removal working across the network
</commit_message>
<xml_diff>
--- a/CardCheckOff.xlsx
+++ b/CardCheckOff.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Documents\GitHub\RIT-Resilience-Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3B50B2-4F11-41F1-8E7F-84DC0FBB24F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83681357-13A7-4BBC-B534-967671420FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="34240" windowHeight="20960" xr2:uid="{64B1DE55-618D-485E-BD09-95462C47B966}"/>
+    <workbookView xWindow="2200" yWindow="450" windowWidth="34240" windowHeight="20530" xr2:uid="{64B1DE55-618D-485E-BD09-95462C47B966}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -663,7 +663,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -955,10 +955,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
         <v>65</v>
@@ -1034,7 +1034,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>30</v>

</xml_diff>